<commit_message>
tried to change the Display.plot_dataframe
</commit_message>
<xml_diff>
--- a/0_Excels/Prob(D_i=d).xlsx
+++ b/0_Excels/Prob(D_i=d).xlsx
@@ -1,34 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kilian\Documents\Schule\2023_24\02_W-Sem M\4 Code\Python\BenfordsLaw\0_Excels\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D84AE75-7AE0-4CEA-86D6-0E8EFB964DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,81 +50,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,145 +355,153 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="B2:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2">
-      <c r="B2" t="n">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B2" s="2">
         <v>0</v>
       </c>
-      <c r="C2" t="n">
-        <v>30.10299956639812</v>
-      </c>
-      <c r="D2" t="n">
-        <v>17.60912590556812</v>
-      </c>
-      <c r="E2" t="n">
-        <v>12.49387366082999</v>
-      </c>
-      <c r="F2" t="n">
-        <v>9.691001300805642</v>
-      </c>
-      <c r="G2" t="n">
-        <v>7.918124604762482</v>
-      </c>
-      <c r="H2" t="n">
-        <v>6.694678963061322</v>
-      </c>
-      <c r="I2" t="n">
+      <c r="C2" s="1">
+        <v>11.967926859688079</v>
+      </c>
+      <c r="D2" s="1">
+        <v>10.17843646442167</v>
+      </c>
+      <c r="E2" s="1">
+        <v>10.01761469399356</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="1">
+        <v>30.102999566398118</v>
+      </c>
+      <c r="C3" s="1">
+        <v>11.38901034075564</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10.13759774478013</v>
+      </c>
+      <c r="E3" s="1">
+        <v>10.013688811757801</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="1">
+        <v>17.609125905568121</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10.88214990055082</v>
+      </c>
+      <c r="D4" s="1">
+        <v>10.09721981370417</v>
+      </c>
+      <c r="E4" s="1">
+        <v>10.009767259461491</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="1">
+        <v>12.493873660829991</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10.43295602309594</v>
+      </c>
+      <c r="D5" s="1">
+        <v>10.05729321109262</v>
+      </c>
+      <c r="E5" s="1">
+        <v>10.005850028348689</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="1">
+        <v>9.6910013008056417</v>
+      </c>
+      <c r="C6" s="1">
+        <v>10.030820226757941</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10.017808762794759</v>
+      </c>
+      <c r="E6" s="1">
+        <v>10.00193710969045</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="1">
+        <v>7.9181246047624816</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9.6677235802322432</v>
+      </c>
+      <c r="D7" s="1">
+        <v>9.9787575692177413</v>
+      </c>
+      <c r="E7" s="1">
+        <v>9.9980284947840996</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="1">
+        <v>6.6946789630613219</v>
+      </c>
+      <c r="C8" s="1">
+        <v>9.3374735783036158</v>
+      </c>
+      <c r="D8" s="1">
+        <v>9.940130994496176</v>
+      </c>
+      <c r="E8" s="1">
+        <v>9.9941241749526029</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="1">
         <v>5.799194697768673</v>
       </c>
-      <c r="J2" t="n">
-        <v>5.115252244738129</v>
-      </c>
-      <c r="K2" t="n">
-        <v>4.575749056067514</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="n">
-        <v>11.96792685968808</v>
-      </c>
-      <c r="C3" t="n">
-        <v>11.38901034075564</v>
-      </c>
-      <c r="D3" t="n">
-        <v>10.88214990055082</v>
-      </c>
-      <c r="E3" t="n">
-        <v>10.43295602309594</v>
-      </c>
-      <c r="F3" t="n">
-        <v>10.03082022675794</v>
-      </c>
-      <c r="G3" t="n">
-        <v>9.667723580232243</v>
-      </c>
-      <c r="H3" t="n">
-        <v>9.337473578303616</v>
-      </c>
-      <c r="I3" t="n">
-        <v>9.035198926960332</v>
-      </c>
-      <c r="J3" t="n">
+      <c r="C9" s="1">
+        <v>9.0351989269603319</v>
+      </c>
+      <c r="D9" s="1">
+        <v>9.9019206561895992</v>
+      </c>
+      <c r="E9" s="1">
+        <v>9.990224141544914</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="1">
+        <v>5.1152522447381292</v>
+      </c>
+      <c r="C10" s="1">
         <v>8.757005357886138</v>
       </c>
-      <c r="K3" t="n">
-        <v>8.499735205769223</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="n">
-        <v>10.17843646442167</v>
-      </c>
-      <c r="C4" t="n">
-        <v>10.13759774478013</v>
-      </c>
-      <c r="D4" t="n">
-        <v>10.09721981370417</v>
-      </c>
-      <c r="E4" t="n">
-        <v>10.05729321109262</v>
-      </c>
-      <c r="F4" t="n">
-        <v>10.01780876279476</v>
-      </c>
-      <c r="G4" t="n">
-        <v>9.978757569217741</v>
-      </c>
-      <c r="H4" t="n">
-        <v>9.940130994496176</v>
-      </c>
-      <c r="I4" t="n">
-        <v>9.901920656189599</v>
-      </c>
-      <c r="J4" t="n">
-        <v>9.864118415477721</v>
-      </c>
-      <c r="K4" t="n">
-        <v>9.826716367825329</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="n">
-        <v>10.01761469399356</v>
-      </c>
-      <c r="C5" t="n">
-        <v>10.0136888117578</v>
-      </c>
-      <c r="D5" t="n">
-        <v>10.00976725946149</v>
-      </c>
-      <c r="E5" t="n">
-        <v>10.00585002834869</v>
-      </c>
-      <c r="F5" t="n">
-        <v>10.00193710969045</v>
-      </c>
-      <c r="G5" t="n">
-        <v>9.9980284947841</v>
-      </c>
-      <c r="H5" t="n">
-        <v>9.994124174952603</v>
-      </c>
-      <c r="I5" t="n">
-        <v>9.990224141544914</v>
-      </c>
-      <c r="J5" t="n">
-        <v>9.986328385937243</v>
-      </c>
-      <c r="K5" t="n">
-        <v>9.982436899529127</v>
+      <c r="D10" s="1">
+        <v>9.8641184154777211</v>
+      </c>
+      <c r="E10" s="1">
+        <v>9.9863283859372434</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="1">
+        <v>4.5757490560675143</v>
+      </c>
+      <c r="C11" s="1">
+        <v>8.4997352057692233</v>
+      </c>
+      <c r="D11" s="1">
+        <v>9.8267163678253286</v>
+      </c>
+      <c r="E11" s="1">
+        <v>9.9824368995291266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>